<commit_message>
Today's commit(01/08/2019) Updated the Data provider code
</commit_message>
<xml_diff>
--- a/src/test/resources/ICAAutomation.xlsx
+++ b/src/test/resources/ICAAutomation.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Udhaya\Eclipse-workspace new\ICAAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED893D6-B644-40A4-A1D6-AF580BC7C823}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E639FD50-0029-418C-A7C3-F2D66D5D56C4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testsheet" sheetId="2" r:id="rId1"/>
+    <sheet name="industrialInjuryFormValidation" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>TCID</t>
   </si>
@@ -705,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BD2"/>
+  <dimension ref="A1:BB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,9 +763,10 @@
     <col min="54" max="54" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="30" customWidth="1"/>
     <col min="56" max="56" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -927,14 +929,8 @@
       <c r="BB1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="BC1" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="BD1" s="4" t="s">
-        <v>90</v>
-      </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1096,12 +1092,6 @@
       </c>
       <c r="BB2" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="BC2" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="BD2" s="7" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1112,4 +1102,52 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59525ACD-6D1A-4AAC-9AA5-5BEEF0A6D5D0}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Today's commit(01/25/2019) Updated code
</commit_message>
<xml_diff>
--- a/src/test/resources/ICAAutomation.xlsx
+++ b/src/test/resources/ICAAutomation.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Udhaya\Eclipse-workspace new\ICAAutomation\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C9367A-A0BA-41E3-9056-FB2324D26983}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{292B22C7-CEB4-450A-9508-2D898932656C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="5835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testsheet" sheetId="2" r:id="rId1"/>
     <sheet name="industrialInjuryFormValidation" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -708,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59525ACD-6D1A-4AAC-9AA5-5BEEF0A6D5D0}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>